<commit_message>
modified dataEnconder check the new Dataset(1)
</commit_message>
<xml_diff>
--- a/code/encoded_data.xlsx
+++ b/code/encoded_data.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaser\Desktop\repo\Course-Recommendation-System\code\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94EDD44-9B59-4284-B8B7-623F20144B2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>Student ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Course ID</t>
   </si>
   <si>
-    <t>Attepmpts</t>
-  </si>
-  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -43,6 +43,9 @@
     <t>Related Topic_5.0</t>
   </si>
   <si>
+    <t>Related Topic_6.0</t>
+  </si>
+  <si>
     <t>Related Topic_7.0</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t>Related Subject_3.0</t>
   </si>
   <si>
+    <t>Related Subject_4.0</t>
+  </si>
+  <si>
     <t>Related Subject_5.0</t>
   </si>
   <si>
@@ -73,18 +79,33 @@
     <t>Related Subject_7.0</t>
   </si>
   <si>
+    <t>Related Subject_8.0</t>
+  </si>
+  <si>
     <t>Related Subject_9.0</t>
   </si>
   <si>
+    <t>Related Subject_10.0</t>
+  </si>
+  <si>
+    <t>Related Subject_11.0</t>
+  </si>
+  <si>
     <t>Related Subject_12.0</t>
   </si>
   <si>
+    <t>Related Subject_13.0</t>
+  </si>
+  <si>
     <t>Related Subject_14.0</t>
   </si>
   <si>
     <t>Related Subject_15.0</t>
   </si>
   <si>
+    <t>Related Subject_16.0</t>
+  </si>
+  <si>
     <t>Related Subject_17.0</t>
   </si>
   <si>
@@ -97,10 +118,16 @@
     <t>Related Subject_20.0</t>
   </si>
   <si>
+    <t>Related Subject_21.0</t>
+  </si>
+  <si>
+    <t>Related Subject_22.0</t>
+  </si>
+  <si>
     <t>Related Subject_23.0</t>
   </si>
   <si>
-    <t>Related Subject_25.0</t>
+    <t>Related Subject_24.0</t>
   </si>
   <si>
     <t>Skill_1.0</t>
@@ -139,8 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +230,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -249,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,9 +316,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,6 +368,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,14 +561,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AV23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,8 +691,29 @@
       <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -627,19 +721,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -648,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -663,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -684,25 +778,25 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -720,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2">
         <v>0</v>
@@ -743,46 +837,67 @@
       <c r="AO2">
         <v>1</v>
       </c>
+      <c r="AP2">
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>1</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -806,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -827,19 +942,19 @@
         <v>1</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE3">
         <v>0</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -863,36 +978,57 @@
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO3">
         <v>1</v>
       </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>2.3</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -931,13 +1067,13 @@
         <v>1</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -949,13 +1085,13 @@
         <v>0</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -976,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4">
         <v>0</v>
@@ -988,51 +1124,72 @@
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>1</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3.080000000000001</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>3.3</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1047,10 +1204,10 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -1068,13 +1225,13 @@
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -1089,13 +1246,13 @@
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5">
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5">
         <v>1</v>
@@ -1110,42 +1267,63 @@
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1154,40 +1332,40 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1202,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1223,42 +1401,63 @@
         <v>0</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM6">
         <v>1</v>
       </c>
       <c r="AN6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO6">
         <v>0</v>
       </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>2.85</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1.7</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1267,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1285,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -1294,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1303,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1330,28 +1529,28 @@
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7">
         <v>0</v>
       </c>
       <c r="AE7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7">
         <v>0</v>
@@ -1360,39 +1559,60 @@
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN7">
         <v>0</v>
       </c>
       <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <v>1</v>
+      </c>
+      <c r="AV7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>3.5</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>2.7</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1407,22 +1627,22 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -1437,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1455,19 +1675,19 @@
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8">
         <v>0</v>
@@ -1476,10 +1696,10 @@
         <v>1</v>
       </c>
       <c r="AJ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8">
         <v>0</v>
@@ -1491,24 +1711,45 @@
         <v>0</v>
       </c>
       <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+      <c r="AU8">
+        <v>1</v>
+      </c>
+      <c r="AV8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>2.5</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1520,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1538,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1562,16 +1803,16 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <v>1</v>
       </c>
       <c r="Y9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -1592,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <v>0</v>
@@ -1607,48 +1848,69 @@
         <v>0</v>
       </c>
       <c r="AL9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM9">
         <v>0</v>
       </c>
       <c r="AN9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO9">
         <v>1</v>
       </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <v>1</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>2.85</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1663,22 +1925,22 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1705,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="AC10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10">
         <v>0</v>
@@ -1717,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <v>0</v>
@@ -1732,16 +1994,1935 @@
         <v>0</v>
       </c>
       <c r="AL10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN10">
         <v>0</v>
       </c>
       <c r="AO10">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>1</v>
+      </c>
+      <c r="AU10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1.65</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>1</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
+      <c r="AR12">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+      <c r="AR13">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>1</v>
+      </c>
+      <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>1</v>
+      </c>
+      <c r="AV13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>2.1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>1</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>1</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>1.3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>1</v>
+      </c>
+      <c r="AU15">
+        <v>0</v>
+      </c>
+      <c r="AV15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>1</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+      <c r="AU16">
+        <v>1</v>
+      </c>
+      <c r="AV16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>1.3</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>1</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>2.5</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>1</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>1</v>
+      </c>
+      <c r="AV18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AM19">
+        <v>1</v>
+      </c>
+      <c r="AN19">
+        <v>1</v>
+      </c>
+      <c r="AO19">
+        <v>1</v>
+      </c>
+      <c r="AP19">
+        <v>1</v>
+      </c>
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+      <c r="AR19">
+        <v>1</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19">
+        <v>0</v>
+      </c>
+      <c r="AV19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20">
+        <v>0</v>
+      </c>
+      <c r="AR20">
+        <v>0</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>1</v>
+      </c>
+      <c r="AU20">
+        <v>1</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>3.7</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
+      </c>
+      <c r="AR21">
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+      <c r="AT21">
+        <v>0</v>
+      </c>
+      <c r="AU21">
+        <v>0</v>
+      </c>
+      <c r="AV21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>3.3</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
+        <v>1</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22">
+        <v>0</v>
+      </c>
+      <c r="AR22">
+        <v>0</v>
+      </c>
+      <c r="AS22">
+        <v>0</v>
+      </c>
+      <c r="AT22">
+        <v>0</v>
+      </c>
+      <c r="AU22">
+        <v>1</v>
+      </c>
+      <c r="AV22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>2.15</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>1</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>1</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>